<commit_message>
Chnages made after adding Tengah and removing IMH
</commit_message>
<xml_diff>
--- a/SG Public Hospitals & Polyclinics.xlsx
+++ b/SG Public Hospitals & Polyclinics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paridhiagarwal/dse3101-LTAProject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dawnk\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9E7AC8-9703-824C-8D68-2301FCB9EB44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90967A79-7718-469E-AF41-5F452C3099F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="39">
   <si>
     <t>Healthcare Facility</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>CHANGI GENERAL HOSPITAL</t>
-  </si>
-  <si>
-    <t>INSTITUTE OF MENTAL HEALTH</t>
   </si>
   <si>
     <t>KHOO TECK PUAT HOSPITAL</t>
@@ -510,21 +507,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="46.33203125" customWidth="1"/>
-    <col min="2" max="2" width="41.83203125" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" customWidth="1"/>
-    <col min="4" max="4" width="36.6640625" customWidth="1"/>
+    <col min="1" max="1" width="46.36328125" customWidth="1"/>
+    <col min="2" max="2" width="41.81640625" customWidth="1"/>
+    <col min="3" max="3" width="24.6328125" customWidth="1"/>
+    <col min="4" max="4" width="36.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -538,7 +535,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -549,10 +546,10 @@
         <v>103.80252400000001</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -563,455 +560,441 @@
         <v>103.94990799999999</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4">
-        <v>1.3821110000000001</v>
+        <v>1.4245699999999999</v>
       </c>
       <c r="C4">
-        <v>103.88579900000001</v>
+        <v>103.839433</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5">
-        <v>1.4245699999999999</v>
+        <v>1.3107120000000001</v>
       </c>
       <c r="C5">
-        <v>103.839433</v>
+        <v>103.84706199999999</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6">
-        <v>1.3107120000000001</v>
+        <v>1.2940640000000001</v>
       </c>
       <c r="C6">
-        <v>103.84706199999999</v>
+        <v>103.782751</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7">
-        <v>1.2940640000000001</v>
+        <v>1.334271</v>
       </c>
       <c r="C7">
-        <v>103.782751</v>
+        <v>103.744626</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8">
-        <v>1.334271</v>
+        <v>1.3955679999999999</v>
       </c>
       <c r="C8">
-        <v>103.744626</v>
+        <v>103.894595</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9">
-        <v>1.3955679999999999</v>
+        <v>1.2796730000000001</v>
       </c>
       <c r="C9">
-        <v>103.894595</v>
+        <v>103.836669</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10">
-        <v>1.2796730000000001</v>
+        <v>1.3215710000000001</v>
       </c>
       <c r="C10">
-        <v>103.836669</v>
+        <v>103.845849</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11">
-        <v>1.3215710000000001</v>
+        <v>1.425362</v>
       </c>
       <c r="C11">
-        <v>103.845849</v>
+        <v>103.79560600000001</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12">
-        <v>1.425362</v>
+        <v>1.316859</v>
       </c>
       <c r="C12">
-        <v>103.79560600000001</v>
+        <v>103.859038</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>15</v>
       </c>
       <c r="B13">
-        <v>1.316859</v>
+        <v>1.4183650000000001</v>
       </c>
       <c r="C13">
-        <v>103.859038</v>
+        <v>103.83437499999999</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>16</v>
       </c>
       <c r="B14">
-        <v>1.4183650000000001</v>
+        <v>1.4481170000000001</v>
       </c>
       <c r="C14">
-        <v>103.83437499999999</v>
+        <v>103.822965</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>17</v>
       </c>
       <c r="B15">
-        <v>1.4481170000000001</v>
+        <v>1.3745099999999999</v>
       </c>
       <c r="C15">
-        <v>103.822965</v>
+        <v>103.84582</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>18</v>
       </c>
       <c r="B16">
-        <v>1.3745099999999999</v>
+        <v>1.3196110000000001</v>
       </c>
       <c r="C16">
-        <v>103.84582</v>
+        <v>103.887229</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>19</v>
       </c>
       <c r="B17">
-        <v>1.3196110000000001</v>
+        <v>1.370231</v>
       </c>
       <c r="C17">
-        <v>103.887229</v>
+        <v>103.889319</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>20</v>
       </c>
       <c r="B18">
-        <v>1.370231</v>
+        <v>1.3347960000000001</v>
       </c>
       <c r="C18">
-        <v>103.889319</v>
+        <v>103.858977</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>21</v>
       </c>
       <c r="B19">
-        <v>1.3347960000000001</v>
+        <v>1.4310259999999999</v>
       </c>
       <c r="C19">
-        <v>103.858977</v>
+        <v>103.77606400000001</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>22</v>
       </c>
       <c r="B20">
-        <v>1.4310259999999999</v>
+        <v>1.4305829999999999</v>
       </c>
       <c r="C20">
-        <v>103.77606400000001</v>
+        <v>103.840191</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>23</v>
       </c>
       <c r="B21">
-        <v>1.4305829999999999</v>
+        <v>1.3274429999999999</v>
       </c>
       <c r="C21">
-        <v>103.840191</v>
+        <v>103.932362</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>24</v>
       </c>
       <c r="B22">
-        <v>1.3274429999999999</v>
+        <v>1.284206</v>
       </c>
       <c r="C22">
-        <v>103.932362</v>
+        <v>103.817674</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>25</v>
       </c>
       <c r="B23">
-        <v>1.284206</v>
+        <v>1.3026150000000001</v>
       </c>
       <c r="C23">
-        <v>103.817674</v>
+        <v>103.908394</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>26</v>
       </c>
       <c r="B24">
-        <v>1.3026150000000001</v>
+        <v>1.2799849999999999</v>
       </c>
       <c r="C24">
-        <v>103.908394</v>
+        <v>103.83916000000001</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>27</v>
       </c>
       <c r="B25">
-        <v>1.2799849999999999</v>
+        <v>1.3736740000000001</v>
       </c>
       <c r="C25">
-        <v>103.83916000000001</v>
+        <v>103.94833199999999</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>28</v>
       </c>
       <c r="B26">
-        <v>1.3736740000000001</v>
+        <v>1.3929450000000001</v>
       </c>
       <c r="C26">
-        <v>103.94833199999999</v>
+        <v>103.895375</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>29</v>
       </c>
       <c r="B27">
-        <v>1.3929450000000001</v>
+        <v>1.357631</v>
       </c>
       <c r="C27">
-        <v>103.895375</v>
+        <v>103.94611399999999</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>30</v>
       </c>
       <c r="B28">
-        <v>1.357631</v>
+        <v>1.3521609999999999</v>
       </c>
       <c r="C28">
-        <v>103.94611399999999</v>
+        <v>103.748974</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>31</v>
       </c>
       <c r="B29">
-        <v>1.3521609999999999</v>
+        <v>1.383194</v>
       </c>
       <c r="C29">
-        <v>103.748974</v>
+        <v>103.76097300000001</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>32</v>
       </c>
       <c r="B30">
-        <v>1.383194</v>
+        <v>1.3823559999999999</v>
       </c>
       <c r="C30">
-        <v>103.76097300000001</v>
+        <v>103.752076</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>33</v>
       </c>
       <c r="B31">
-        <v>1.3823559999999999</v>
+        <v>1.312991</v>
       </c>
       <c r="C31">
-        <v>103.752076</v>
+        <v>103.765878</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>34</v>
       </c>
       <c r="B32">
-        <v>1.312991</v>
+        <v>1.3501890000000001</v>
       </c>
       <c r="C32">
-        <v>103.765878</v>
+        <v>103.730642</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>35</v>
       </c>
       <c r="B33">
-        <v>1.3501890000000001</v>
+        <v>1.338732</v>
       </c>
       <c r="C33">
-        <v>103.730642</v>
+        <v>103.700228</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>36</v>
       </c>
       <c r="B34">
-        <v>1.338732</v>
+        <v>1.298751</v>
       </c>
       <c r="C34">
-        <v>103.700228</v>
+        <v>103.801618</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35">
-        <v>1.298751</v>
-      </c>
-      <c r="C35">
-        <v>103.801618</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>